<commit_message>
Handled nulls and divide by zero errors, enhanced tests.
</commit_message>
<xml_diff>
--- a/src/main/resources/Employee Data.xlsx
+++ b/src/main/resources/Employee Data.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adponlineind-my.sharepoint.com/personal/sharmav2_es_ad_adp_com/Documents/ADP/Code/mine/employee-management/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{D80233B7-F55C-4736-966E-AEE9FD0B066B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16043F6A-0E37-41FE-8984-673FA7C6B36A}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_F25DC773A252ABDACC10484F091D54B65ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04685F37-EBC7-407A-BAC8-6D0F16192A4B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CA36995C-0FBA-4DF0-9682-F42E048FCEDB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -91,7 +80,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -116,9 +105,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -151,39 +139,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -216,26 +204,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -268,23 +239,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -346,6 +300,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -354,13 +315,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -425,47 +379,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAC5426-52BA-452A-B9EE-CF77A84D0A11}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,14 +415,8 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="J1" s="1">
-        <v>1.5</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>123</v>
       </c>
@@ -501,19 +429,8 @@
       <c r="D2">
         <v>60000</v>
       </c>
-      <c r="H2">
-        <v>46000</v>
-      </c>
-      <c r="I2">
-        <f>H2*1.2</f>
-        <v>55200</v>
-      </c>
-      <c r="J2">
-        <f>I2*1.5</f>
-        <v>82800</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>124</v>
       </c>
@@ -529,19 +446,8 @@
       <c r="E3">
         <v>123</v>
       </c>
-      <c r="H3">
-        <v>50000</v>
-      </c>
-      <c r="I3">
-        <f>H3*1.2</f>
-        <v>60000</v>
-      </c>
-      <c r="J3">
-        <f>I3*1.5</f>
-        <v>90000</v>
-      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>125</v>
       </c>
@@ -557,19 +463,8 @@
       <c r="E4">
         <v>123</v>
       </c>
-      <c r="H4">
-        <v>34000</v>
-      </c>
-      <c r="I4">
-        <f>H4*1.2</f>
-        <v>40800</v>
-      </c>
-      <c r="J4">
-        <f>I4*1.5</f>
-        <v>61200</v>
-      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>300</v>
       </c>
@@ -586,7 +481,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>305</v>
       </c>

</xml_diff>

<commit_message>
Updated logic with rounding of %age
</commit_message>
<xml_diff>
--- a/src/main/resources/Employee Data.xlsx
+++ b/src/main/resources/Employee Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adponlineind-my.sharepoint.com/personal/sharmav2_es_ad_adp_com/Documents/ADP/Code/mine/employee-management/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_F25DC773A252ABDACC10484F091D54B65ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04685F37-EBC7-407A-BAC8-6D0F16192A4B}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="11_F25DC773A252ABDACC10484F091D54B65ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86E3E9D8-F739-412F-BE88-88E48948BB91}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Id</t>
   </si>
@@ -70,6 +70,54 @@
   </si>
   <si>
     <t>Hardleaf</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Tony</t>
+  </si>
+  <si>
+    <t>Stark</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Rogers</t>
+  </si>
+  <si>
+    <t>Natasha</t>
+  </si>
+  <si>
+    <t>Romanoff</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Fury</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Strange</t>
+  </si>
+  <si>
+    <t>Bruce</t>
+  </si>
+  <si>
+    <t>Banner</t>
   </si>
 </sst>
 </file>
@@ -391,13 +439,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -498,6 +549,142 @@
         <v>300</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>306</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>40000</v>
+      </c>
+      <c r="E7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>307</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>50000</v>
+      </c>
+      <c r="E8">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>308</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>70000</v>
+      </c>
+      <c r="E9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>310</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>40000</v>
+      </c>
+      <c r="E10">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>311</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>45000</v>
+      </c>
+      <c r="E11">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>450</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>50000</v>
+      </c>
+      <c r="E12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>353</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>35000</v>
+      </c>
+      <c r="E13">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>367</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>40000</v>
+      </c>
+      <c r="E14">
+        <v>450</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed from Excel Reader to CSV Reader and the subsequent tests
</commit_message>
<xml_diff>
--- a/src/main/resources/Employee Data.xlsx
+++ b/src/main/resources/Employee Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adponlineind-my.sharepoint.com/personal/sharmav2_es_ad_adp_com/Documents/ADP/Code/mine/employee-management/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_F25DC773A252ABDACC10484F091D54B65ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86E3E9D8-F739-412F-BE88-88E48948BB91}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_F25DC773A252ABDACC10484F091D54B65ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB2D411B-A815-4144-AEF7-CDD60016C678}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Id</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Banner</t>
+  </si>
+  <si>
+    <t>Hank</t>
+  </si>
+  <si>
+    <t>Pym</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,6 +691,23 @@
         <v>450</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>451</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>35000</v>
+      </c>
+      <c r="E15">
+        <v>311</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>